<commit_message>
updated 3 dpf data
</commit_message>
<xml_diff>
--- a/DataSheets/Timeline_mbpcaaxnls.xlsx
+++ b/DataSheets/Timeline_mbpcaaxnls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miramota/Desktop/Graphs/DataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD8221F-412B-664A-B9D6-7FECDCBD002F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D5A54B-A908-1148-978F-A0C05C4D2415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{071ECDE8-A980-C64F-9A21-20281849EC54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{071ECDE8-A980-C64F-9A21-20281849EC54}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="119">
   <si>
     <t>aberrant</t>
   </si>
@@ -333,13 +333,73 @@
   </si>
   <si>
     <t>DDD</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>apricot</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>blackberry</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>cherry</t>
+  </si>
+  <si>
+    <t>clementine</t>
+  </si>
+  <si>
+    <t>cranberry</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>grapes</t>
+  </si>
+  <si>
+    <t>grapefruit</t>
+  </si>
+  <si>
+    <t>guava</t>
+  </si>
+  <si>
+    <t>durian</t>
+  </si>
+  <si>
+    <t>fig</t>
+  </si>
+  <si>
+    <t>honeydew</t>
+  </si>
+  <si>
+    <t>kiwi</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>mango</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -359,6 +419,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -430,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -442,6 +514,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDC249E-7F27-2843-A738-2890B36CAB9D}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="K129" sqref="K129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2933,7 +3006,815 @@
         <v>44</v>
       </c>
     </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11">
+        <v>0</v>
+      </c>
+      <c r="D94" s="11">
+        <v>3</v>
+      </c>
+      <c r="E94" s="11">
+        <v>0</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11">
+        <v>6</v>
+      </c>
+      <c r="D95" s="11">
+        <v>3</v>
+      </c>
+      <c r="E95" s="11">
+        <v>0</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11">
+        <v>3</v>
+      </c>
+      <c r="D96" s="11">
+        <v>3</v>
+      </c>
+      <c r="E96" s="11">
+        <v>0</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11">
+        <v>0</v>
+      </c>
+      <c r="D97" s="11">
+        <v>3</v>
+      </c>
+      <c r="E97" s="11">
+        <v>0</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11">
+        <v>1</v>
+      </c>
+      <c r="D98" s="11">
+        <v>3</v>
+      </c>
+      <c r="E98" s="11">
+        <v>0</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11">
+        <v>2</v>
+      </c>
+      <c r="D99" s="11">
+        <v>3</v>
+      </c>
+      <c r="E99" s="11">
+        <v>0</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11">
+        <v>2</v>
+      </c>
+      <c r="D100" s="11">
+        <v>3</v>
+      </c>
+      <c r="E100" s="11">
+        <v>0</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11">
+        <v>0</v>
+      </c>
+      <c r="D101" s="11">
+        <v>3</v>
+      </c>
+      <c r="E101" s="11">
+        <v>0</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11">
+        <v>1</v>
+      </c>
+      <c r="D102" s="11">
+        <v>3</v>
+      </c>
+      <c r="E102" s="11">
+        <v>0</v>
+      </c>
+      <c r="F102" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11">
+        <v>2</v>
+      </c>
+      <c r="D103" s="11">
+        <v>3</v>
+      </c>
+      <c r="E103" s="11">
+        <v>0</v>
+      </c>
+      <c r="F103" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G103" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" s="11"/>
+      <c r="C104" s="11">
+        <v>0</v>
+      </c>
+      <c r="D104" s="11">
+        <v>3</v>
+      </c>
+      <c r="E104" s="11">
+        <v>0</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11">
+        <v>0</v>
+      </c>
+      <c r="D105" s="11">
+        <v>3</v>
+      </c>
+      <c r="E105" s="11">
+        <v>0</v>
+      </c>
+      <c r="F105" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G105" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11">
+        <v>1</v>
+      </c>
+      <c r="D106" s="11">
+        <v>3</v>
+      </c>
+      <c r="E106" s="11">
+        <v>0</v>
+      </c>
+      <c r="F106" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11">
+        <v>2</v>
+      </c>
+      <c r="D107" s="11">
+        <v>3</v>
+      </c>
+      <c r="E107" s="11">
+        <v>0</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11">
+        <v>4</v>
+      </c>
+      <c r="D108" s="11">
+        <v>3</v>
+      </c>
+      <c r="E108" s="11">
+        <v>0</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11">
+        <v>2</v>
+      </c>
+      <c r="D109" s="11">
+        <v>3</v>
+      </c>
+      <c r="E109" s="11">
+        <v>0</v>
+      </c>
+      <c r="F109" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G109" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11">
+        <v>0</v>
+      </c>
+      <c r="D110" s="11">
+        <v>3</v>
+      </c>
+      <c r="E110" s="11">
+        <v>0</v>
+      </c>
+      <c r="F110" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G110" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B111" s="11"/>
+      <c r="C111" s="11">
+        <v>0</v>
+      </c>
+      <c r="D111" s="11">
+        <v>3</v>
+      </c>
+      <c r="E111" s="11">
+        <v>0</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11">
+        <v>0</v>
+      </c>
+      <c r="D112" s="11">
+        <v>3</v>
+      </c>
+      <c r="E112" s="11">
+        <v>0</v>
+      </c>
+      <c r="F112" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11">
+        <v>0</v>
+      </c>
+      <c r="D113" s="11">
+        <v>4</v>
+      </c>
+      <c r="E113" s="11">
+        <v>0</v>
+      </c>
+      <c r="F113" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11">
+        <v>8</v>
+      </c>
+      <c r="D114" s="11">
+        <v>4</v>
+      </c>
+      <c r="E114" s="11">
+        <v>0</v>
+      </c>
+      <c r="F114" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" s="11"/>
+      <c r="C115" s="11">
+        <v>5</v>
+      </c>
+      <c r="D115" s="11">
+        <v>4</v>
+      </c>
+      <c r="E115" s="11">
+        <v>0</v>
+      </c>
+      <c r="F115" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B116" s="11"/>
+      <c r="C116" s="11">
+        <v>0</v>
+      </c>
+      <c r="D116" s="11">
+        <v>4</v>
+      </c>
+      <c r="E116" s="11">
+        <v>0</v>
+      </c>
+      <c r="F116" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B117" s="11"/>
+      <c r="C117" s="11">
+        <v>2</v>
+      </c>
+      <c r="D117" s="11">
+        <v>4</v>
+      </c>
+      <c r="E117" s="11">
+        <v>0</v>
+      </c>
+      <c r="F117" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B118" s="11"/>
+      <c r="C118" s="11">
+        <v>2</v>
+      </c>
+      <c r="D118" s="11">
+        <v>4</v>
+      </c>
+      <c r="E118" s="11">
+        <v>0</v>
+      </c>
+      <c r="F118" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B119" s="11"/>
+      <c r="C119" s="11">
+        <v>1</v>
+      </c>
+      <c r="D119" s="11">
+        <v>4</v>
+      </c>
+      <c r="E119" s="11">
+        <v>0</v>
+      </c>
+      <c r="F119" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11">
+        <v>3</v>
+      </c>
+      <c r="D120" s="11">
+        <v>4</v>
+      </c>
+      <c r="E120" s="11">
+        <v>0</v>
+      </c>
+      <c r="F120" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11">
+        <v>2</v>
+      </c>
+      <c r="D121" s="11">
+        <v>4</v>
+      </c>
+      <c r="E121" s="11">
+        <v>0</v>
+      </c>
+      <c r="F121" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11">
+        <v>4</v>
+      </c>
+      <c r="D122" s="11">
+        <v>4</v>
+      </c>
+      <c r="E122" s="11">
+        <v>0</v>
+      </c>
+      <c r="F122" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B123" s="11"/>
+      <c r="C123" s="11">
+        <v>0</v>
+      </c>
+      <c r="D123" s="11">
+        <v>4</v>
+      </c>
+      <c r="E123" s="11">
+        <v>0</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11">
+        <v>0</v>
+      </c>
+      <c r="D124" s="11">
+        <v>4</v>
+      </c>
+      <c r="E124" s="11">
+        <v>0</v>
+      </c>
+      <c r="F124" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11">
+        <v>2</v>
+      </c>
+      <c r="D125" s="11">
+        <v>4</v>
+      </c>
+      <c r="E125" s="11">
+        <v>1</v>
+      </c>
+      <c r="F125" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11">
+        <v>1</v>
+      </c>
+      <c r="D126" s="11">
+        <v>4</v>
+      </c>
+      <c r="E126" s="11">
+        <v>1</v>
+      </c>
+      <c r="F126" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11">
+        <v>10</v>
+      </c>
+      <c r="D127" s="11">
+        <v>4</v>
+      </c>
+      <c r="E127" s="11">
+        <v>1</v>
+      </c>
+      <c r="F127" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11">
+        <v>0</v>
+      </c>
+      <c r="D128" s="11">
+        <v>4</v>
+      </c>
+      <c r="E128" s="11">
+        <v>1</v>
+      </c>
+      <c r="F128" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11">
+        <v>0</v>
+      </c>
+      <c r="D129" s="11">
+        <v>4</v>
+      </c>
+      <c r="E129" s="11">
+        <v>1</v>
+      </c>
+      <c r="F129" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B130" s="11"/>
+      <c r="C130" s="11">
+        <v>6</v>
+      </c>
+      <c r="D130" s="11">
+        <v>4</v>
+      </c>
+      <c r="E130" s="11">
+        <v>1</v>
+      </c>
+      <c r="F130" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B131" s="11"/>
+      <c r="C131" s="11">
+        <v>1</v>
+      </c>
+      <c r="D131" s="11">
+        <v>4</v>
+      </c>
+      <c r="E131" s="11">
+        <v>1</v>
+      </c>
+      <c r="F131" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G131" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" s="11"/>
+      <c r="B132" s="11"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>